<commit_message>
add Proj & person_bom
</commit_message>
<xml_diff>
--- a/08_Person Bom Table/myself personal bom.xlsx
+++ b/08_Person Bom Table/myself personal bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="420" windowWidth="20490" windowHeight="7335" tabRatio="842"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="20490" windowHeight="7335" tabRatio="842" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>序号</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -139,10 +139,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>价格(RMB)</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>e-Link32 下载调试器</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -167,11 +163,108 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve"> 探索者 STM32F4</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Micro UNO R3 开发板 改进版 增强版 
+ATmega328P 单片机</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">AVR </t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atmel</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
     <t>frist-4</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> 探索者 STM32F4</t>
+    <t>frist-5</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>戴尔（DELL）</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>深圳海瑟威电子</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPS屏显示器</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>戴尔(P2417好23.8英寸)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>frist-6</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">40 Pin 母对母彩色杜邦线 </t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>价格单价(RMB)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>frist-7</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>frist-8</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>frist-9</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>20cm, 40根一排,
+一头公一头母</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>20cm,40根一排母头</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>20cm,40根一排公头</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">40 Pin 公对母彩色杜邦线 </t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">40 Pin 公对公彩色杜邦线 </t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>匿名科创</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>STM32F407 168MHz
+ICM20602 贯性传感器
+AK8975 高精度气压高度计</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>匿名拓空者飞控+数传 
+送激光定高模块</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -583,7 +676,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -699,21 +792,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -728,67 +806,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -937,93 +954,81 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="48" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1402,250 +1407,250 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="18.25" style="9" customWidth="1"/>
-    <col min="4" max="4" width="27.25" style="9" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="30.75" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="7" customWidth="1"/>
+    <col min="4" max="4" width="27.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="30.75" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="14">
         <v>42996</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="16"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="16"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="16"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="16"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="16"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="16"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="16"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="16"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="16"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -1661,237 +1666,302 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="25" style="9" customWidth="1"/>
-    <col min="5" max="6" width="15.625" style="9"/>
-    <col min="7" max="7" width="15.625" style="7"/>
-    <col min="8" max="8" width="15.625" style="21"/>
-    <col min="9" max="9" width="15.625" style="5"/>
-    <col min="10" max="10" width="19.25" style="7" customWidth="1"/>
+    <col min="1" max="1" width="5.625" customWidth="1"/>
+    <col min="3" max="3" width="25" style="7" customWidth="1"/>
+    <col min="5" max="6" width="15.625" style="7"/>
+    <col min="7" max="7" width="15.625" style="5"/>
+    <col min="8" max="8" width="15.625" style="17"/>
+    <col min="9" max="9" width="15.625" style="3"/>
+    <col min="10" max="10" width="19.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-    </row>
-    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="22"/>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="6">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="16">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="16">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="14">
+      <c r="D5" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="23">
+      <c r="J5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="16">
         <v>1</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="8">
-        <v>482</v>
-      </c>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="20">
+      <c r="I6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="16">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="6">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="20">
+      <c r="I8" s="1"/>
+      <c r="J8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="6">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1"/>
+      <c r="B10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="16">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="6">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1"/>
+      <c r="B11" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="16">
         <v>1</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="20">
-        <v>408</v>
-      </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="20">
-        <v>3</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="20">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="20">
-        <v>39</v>
-      </c>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:12" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7" s="21"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="5"/>
+      <c r="I11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="6">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
@@ -1902,8 +1972,8 @@
       <c r="I12"/>
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:12" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
@@ -1914,8 +1984,8 @@
       <c r="I13"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:12" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
@@ -1926,7 +1996,7 @@
       <c r="I14"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -1938,7 +2008,7 @@
       <c r="I15"/>
       <c r="J15"/>
     </row>
-    <row r="16" spans="1:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1950,7 +2020,7 @@
       <c r="I16"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1962,7 +2032,7 @@
       <c r="I17"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1974,7 +2044,7 @@
       <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1986,7 +2056,7 @@
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1998,7 +2068,7 @@
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -2010,7 +2080,7 @@
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -2022,7 +2092,7 @@
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -2034,7 +2104,7 @@
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -2046,7 +2116,7 @@
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -2058,7 +2128,7 @@
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -2070,7 +2140,7 @@
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -2082,7 +2152,7 @@
       <c r="I27"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -2094,7 +2164,7 @@
       <c r="I28"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -2106,7 +2176,7 @@
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -2118,7 +2188,7 @@
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -2130,7 +2200,7 @@
       <c r="I31"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -2142,7 +2212,7 @@
       <c r="I32"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -2154,7 +2224,7 @@
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -2166,7 +2236,7 @@
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -2178,7 +2248,7 @@
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -2190,7 +2260,7 @@
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -2202,7 +2272,7 @@
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:10" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -2256,9 +2326,14 @@
     <hyperlink ref="J5" r:id="rId1" tooltip="修远智控实验室" display="https://shop113218572.world.taobao.com/"/>
     <hyperlink ref="J3" r:id="rId2" tooltip="修远智控实验室"/>
     <hyperlink ref="J4" r:id="rId3" tooltip="修远智控实验室"/>
+    <hyperlink ref="J7" r:id="rId4"/>
+    <hyperlink ref="J8" r:id="rId5"/>
+    <hyperlink ref="J9" r:id="rId6"/>
+    <hyperlink ref="J10" r:id="rId7"/>
+    <hyperlink ref="J11" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" verticalDpi="1200" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>